<commit_message>
code changes on 05June
</commit_message>
<xml_diff>
--- a/SeleniumMainProject/src/main/resources/TestData.xlsx
+++ b/SeleniumMainProject/src/main/resources/TestData.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerri\git\7rmart_Supermarket\SeleniumMainProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95296A5-1429-4C17-87D5-85DC9B7396DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B43EAC3-74C5-4043-BBE0-7B8B9EF02CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3150" windowWidth="29040" windowHeight="15720" xr2:uid="{8DAAF140-354A-40ED-86C7-24ED4EB653CD}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -423,7 +422,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,16 +458,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EB60F6-0A9B-48DB-AE6B-4D026268DC44}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>